<commit_message>
Starting to work on the second drill
</commit_message>
<xml_diff>
--- a/Lalaon-teny (Ny Tsiory) - Cas.xlsx
+++ b/Lalaon-teny (Ny Tsiory) - Cas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6814F00-7907-4BF3-9B03-728A966B8174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8E59F3-D384-41AE-9F59-546578DD997C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="626" xr2:uid="{27FFEEF4-A9D8-40D1-B209-21085DC60689}"/>
   </bookViews>
@@ -3400,6 +3400,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>78271</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>121635</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1993B5C-5A07-4A0D-3EBC-00A789DDBE43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11382375" y="27360563"/>
+          <a:ext cx="14842021" cy="1371791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>345281</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>586066</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{113DC965-FE8A-5CE8-F020-14AA928A1D3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="559594" y="19812000"/>
+          <a:ext cx="1991003" cy="7060406"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3784,8 +3872,8 @@
   </sheetPr>
   <dimension ref="A1:AT145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A69" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -4984,7 +5072,7 @@
         <v/>
       </c>
       <c r="K69" s="83" t="str">
-        <f t="shared" ref="K69:K70" si="1">_xlfn.TRANSLATE(C69,"fr")</f>
+        <f t="shared" ref="K69" si="1">_xlfn.TRANSLATE(C69,"fr")</f>
         <v>All these letters are obtained after the first 18 tiles.</v>
       </c>
     </row>
@@ -5345,9 +5433,7 @@
       <c r="D78" s="55">
         <v>15</v>
       </c>
-      <c r="E78" s="13">
-        <v>18</v>
-      </c>
+      <c r="E78" s="13"/>
       <c r="F78" s="36"/>
       <c r="G78" s="53" t="s">
         <v>83</v>
@@ -5430,9 +5516,7 @@
       <c r="D79" s="55">
         <v>15</v>
       </c>
-      <c r="E79" s="13">
-        <v>20</v>
-      </c>
+      <c r="E79" s="13"/>
       <c r="F79" s="36"/>
       <c r="G79" s="53" t="s">
         <v>89</v>
@@ -5515,9 +5599,7 @@
       <c r="D80" s="55">
         <v>15</v>
       </c>
-      <c r="E80" s="13">
-        <v>9</v>
-      </c>
+      <c r="E80" s="13"/>
       <c r="F80" s="36"/>
       <c r="G80" s="53" t="s">
         <v>90</v>
@@ -5600,9 +5682,7 @@
       <c r="D81" s="55">
         <v>15</v>
       </c>
-      <c r="E81" s="13">
-        <v>6</v>
-      </c>
+      <c r="E81" s="13"/>
       <c r="F81" s="36"/>
       <c r="G81" s="53" t="s">
         <v>93</v>
@@ -5685,9 +5765,7 @@
       <c r="D82" s="55">
         <v>15</v>
       </c>
-      <c r="E82" s="13">
-        <v>19</v>
-      </c>
+      <c r="E82" s="13"/>
       <c r="F82" s="36"/>
       <c r="G82" s="53" t="s">
         <v>95</v>
@@ -5770,9 +5848,7 @@
       <c r="D83" s="55">
         <v>15</v>
       </c>
-      <c r="E83" s="13">
-        <v>17</v>
-      </c>
+      <c r="E83" s="13"/>
       <c r="F83" s="36"/>
       <c r="G83" s="53" t="s">
         <v>96</v>
@@ -5855,9 +5931,7 @@
       <c r="D84" s="55">
         <v>15</v>
       </c>
-      <c r="E84" s="13">
-        <v>4</v>
-      </c>
+      <c r="E84" s="13"/>
       <c r="F84" s="36"/>
       <c r="G84" s="53" t="s">
         <v>97</v>
@@ -5940,9 +6014,7 @@
       <c r="D85" s="55">
         <v>15</v>
       </c>
-      <c r="E85" s="13">
-        <v>18</v>
-      </c>
+      <c r="E85" s="13"/>
       <c r="F85" s="36"/>
       <c r="G85" s="53" t="s">
         <v>98</v>
@@ -6025,9 +6097,7 @@
       <c r="D86" s="55">
         <v>15</v>
       </c>
-      <c r="E86" s="13">
-        <v>13</v>
-      </c>
+      <c r="E86" s="13"/>
       <c r="F86" s="36"/>
       <c r="G86" s="53" t="s">
         <v>99</v>
@@ -6110,9 +6180,7 @@
       <c r="D87" s="55">
         <v>15</v>
       </c>
-      <c r="E87" s="13">
-        <v>18</v>
-      </c>
+      <c r="E87" s="13"/>
       <c r="F87" s="36"/>
       <c r="G87" s="53" t="s">
         <v>100</v>
@@ -6195,9 +6263,7 @@
       <c r="D88" s="55">
         <v>15</v>
       </c>
-      <c r="E88" s="13">
-        <v>12</v>
-      </c>
+      <c r="E88" s="13"/>
       <c r="F88" s="36"/>
       <c r="G88" s="53" t="s">
         <v>101</v>
@@ -6280,9 +6346,7 @@
       <c r="D89" s="55">
         <v>15</v>
       </c>
-      <c r="E89" s="13">
-        <v>12</v>
-      </c>
+      <c r="E89" s="13"/>
       <c r="F89" s="36"/>
       <c r="G89" s="53" t="s">
         <v>102</v>
@@ -6365,9 +6429,7 @@
       <c r="D90" s="55">
         <v>15</v>
       </c>
-      <c r="E90" s="13">
-        <v>19</v>
-      </c>
+      <c r="E90" s="13"/>
       <c r="F90" s="36"/>
       <c r="G90" s="53" t="s">
         <v>103</v>
@@ -6450,9 +6512,7 @@
       <c r="D91" s="55">
         <v>15</v>
       </c>
-      <c r="E91" s="13">
-        <v>19</v>
-      </c>
+      <c r="E91" s="13"/>
       <c r="F91" s="36"/>
       <c r="G91" s="53" t="s">
         <v>104</v>
@@ -6535,9 +6595,7 @@
       <c r="D92" s="55">
         <v>15</v>
       </c>
-      <c r="E92" s="13">
-        <v>13</v>
-      </c>
+      <c r="E92" s="13"/>
       <c r="F92" s="36"/>
       <c r="G92" s="53" t="s">
         <v>105</v>
@@ -6620,9 +6678,7 @@
       <c r="D93" s="55">
         <v>15</v>
       </c>
-      <c r="E93" s="13">
-        <v>7</v>
-      </c>
+      <c r="E93" s="13"/>
       <c r="F93" s="36"/>
       <c r="G93" s="53" t="s">
         <v>97</v>
@@ -6705,9 +6761,7 @@
       <c r="D94" s="55">
         <v>15</v>
       </c>
-      <c r="E94" s="13">
-        <v>12</v>
-      </c>
+      <c r="E94" s="13"/>
       <c r="F94" s="36"/>
       <c r="G94" s="53" t="s">
         <v>106</v>
@@ -6790,9 +6844,7 @@
       <c r="D95" s="55">
         <v>15</v>
       </c>
-      <c r="E95" s="13">
-        <v>11</v>
-      </c>
+      <c r="E95" s="13"/>
       <c r="F95" s="36"/>
       <c r="G95" s="53" t="s">
         <v>107</v>
@@ -6875,9 +6927,7 @@
       <c r="D96" s="55">
         <v>15</v>
       </c>
-      <c r="E96" s="13">
-        <v>13</v>
-      </c>
+      <c r="E96" s="13"/>
       <c r="F96" s="36"/>
       <c r="G96" s="53" t="s">
         <v>108</v>
@@ -6960,9 +7010,7 @@
       <c r="D97" s="55">
         <v>15</v>
       </c>
-      <c r="E97" s="13">
-        <v>16</v>
-      </c>
+      <c r="E97" s="13"/>
       <c r="F97" s="36"/>
       <c r="G97" s="53" t="s">
         <v>109</v>
@@ -7048,7 +7096,7 @@
       <c r="D99" s="37"/>
       <c r="E99" s="38" t="str">
         <f>IFERROR(E78,"")&amp;";"&amp;IFERROR(E79,"")&amp;";"&amp;IFERROR(E80,"")&amp;";"&amp;IFERROR(E81,"")&amp;";"&amp;IFERROR(E82,"")&amp;";"&amp;IFERROR(E83,"")&amp;";"&amp;IFERROR(E84,"")&amp;";"&amp;IFERROR(E85,"")&amp;";"&amp;IFERROR(E86,"")&amp;";"&amp;IFERROR(E87,"")&amp;";"&amp;IFERROR(E88,"")&amp;";"&amp;IFERROR(E89,"")&amp;";"&amp;IFERROR(E90,"")&amp;";"&amp;IFERROR(E91,"")&amp;";"&amp;IFERROR(E92,"")&amp;";"&amp;IFERROR(E93,"")&amp;";"&amp;IFERROR(E94,"")&amp;";"&amp;IFERROR(E95,"")&amp;";"&amp;IFERROR(E96,"")&amp;";"&amp;IFERROR(E97,"")</f>
-        <v>18;20;9;6;19;17;4;18;13;18;12;12;19;19;13;7;12;11;13;16</v>
+        <v>;;;;;;;;;;;;;;;;;;;</v>
       </c>
       <c r="F99" s="39"/>
       <c r="T99" s="3"/>

</xml_diff>

<commit_message>
Finally beginning to understand the second problem
</commit_message>
<xml_diff>
--- a/Lalaon-teny (Ny Tsiory) - Cas.xlsx
+++ b/Lalaon-teny (Ny Tsiory) - Cas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8E59F3-D384-41AE-9F59-546578DD997C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B047B7F-EB99-43FD-ABDC-658CA9F78DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="626" xr2:uid="{27FFEEF4-A9D8-40D1-B209-21085DC60689}"/>
   </bookViews>
@@ -3408,8 +3408,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>78271</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>423552</xdr:colOff>
       <xdr:row>105</xdr:row>
       <xdr:rowOff>121635</xdr:rowOff>
     </xdr:to>
@@ -3872,8 +3872,8 @@
   </sheetPr>
   <dimension ref="A1:AT145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A69" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E64" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AF76" sqref="AF76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -3894,7 +3894,9 @@
     <col min="22" max="22" width="8.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.5546875" style="3"/>
+    <col min="25" max="31" width="8.5546875" style="3"/>
+    <col min="32" max="51" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="52" max="16384" width="8.5546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="15" customHeight="1">
@@ -5016,11 +5018,11 @@
       </c>
       <c r="K64" s="3"/>
     </row>
-    <row r="65" spans="1:29" ht="15" customHeight="1" thickTop="1">
+    <row r="65" spans="1:32" ht="15" customHeight="1" thickTop="1">
       <c r="A65" s="3"/>
       <c r="K65" s="3"/>
     </row>
-    <row r="66" spans="1:29" ht="15" customHeight="1">
+    <row r="66" spans="1:32" ht="15" customHeight="1">
       <c r="A66" s="3"/>
       <c r="B66" s="11" t="s">
         <v>50</v>
@@ -5032,7 +5034,7 @@
       </c>
       <c r="K66" s="3"/>
     </row>
-    <row r="67" spans="1:29" ht="15" customHeight="1">
+    <row r="67" spans="1:32" ht="15" customHeight="1">
       <c r="A67" s="3"/>
       <c r="B67" s="10"/>
       <c r="G67" s="11"/>
@@ -5042,7 +5044,7 @@
       </c>
       <c r="K67" s="3"/>
     </row>
-    <row r="68" spans="1:29" ht="15" customHeight="1">
+    <row r="68" spans="1:32" ht="15" customHeight="1">
       <c r="A68" s="3"/>
       <c r="B68" s="10" t="s">
         <v>51</v>
@@ -5060,7 +5062,7 @@
         <v>The word HAMIRAPIRATRA requires 1 H tile, 4 A tiles, 1 M tile, 2 I tiles, 3 R tiles, 1 P tile, and 1 T tile.</v>
       </c>
     </row>
-    <row r="69" spans="1:29" ht="15" customHeight="1">
+    <row r="69" spans="1:32" ht="15" customHeight="1">
       <c r="A69" s="3"/>
       <c r="B69" s="10"/>
       <c r="C69" s="15" t="s">
@@ -5076,7 +5078,7 @@
         <v>All these letters are obtained after the first 18 tiles.</v>
       </c>
     </row>
-    <row r="70" spans="1:29" ht="15" customHeight="1">
+    <row r="70" spans="1:32" ht="15" customHeight="1">
       <c r="A70" s="3"/>
       <c r="B70" s="10" t="s">
         <v>54</v>
@@ -5094,7 +5096,7 @@
         <v>The word ITY requires 1 tile of each letter: I, T, and Y.</v>
       </c>
     </row>
-    <row r="71" spans="1:29" ht="15" customHeight="1" thickBot="1">
+    <row r="71" spans="1:32" ht="15" customHeight="1" thickBot="1">
       <c r="A71" s="3"/>
       <c r="B71" s="10"/>
       <c r="C71" s="1" t="s">
@@ -5106,7 +5108,7 @@
         <v>These letters are all joined together through the first 6 tiles.</v>
       </c>
     </row>
-    <row r="72" spans="1:29" ht="15" customHeight="1" thickTop="1" thickBot="1">
+    <row r="72" spans="1:32" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A72" s="3"/>
       <c r="B72" s="10"/>
       <c r="G72" s="11"/>
@@ -5133,7 +5135,7 @@
       <c r="AB72" s="73"/>
       <c r="AC72" s="74"/>
     </row>
-    <row r="73" spans="1:29" ht="24.6" customHeight="1" thickTop="1" thickBot="1">
+    <row r="73" spans="1:32" ht="24.6" customHeight="1" thickTop="1" thickBot="1">
       <c r="A73" s="3"/>
       <c r="B73" s="18" t="s">
         <v>10</v>
@@ -5228,7 +5230,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:29" ht="15" thickTop="1">
+    <row r="74" spans="1:32" ht="15" thickTop="1">
       <c r="A74" s="3"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -5238,7 +5240,7 @@
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
     </row>
-    <row r="75" spans="1:29" ht="24.9" customHeight="1">
+    <row r="75" spans="1:32" ht="24.9" customHeight="1">
       <c r="A75" s="3"/>
       <c r="B75" s="19" t="s">
         <v>59</v>
@@ -5321,8 +5323,12 @@
       <c r="AC75" s="40" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="76" spans="1:29" ht="24.9" customHeight="1">
+      <c r="AF75" s="3" cm="1">
+        <f t="array" ref="AF75">_xlfn.XMATCH(1,_xlfn.SCAN(0,--(J75:AC75="H"),_xleta.SUM))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:32" ht="24.9" customHeight="1">
       <c r="A76" s="3"/>
       <c r="B76" s="19" t="s">
         <v>72</v>
@@ -5406,7 +5412,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:29" ht="15.6">
+    <row r="77" spans="1:32" ht="15.6">
       <c r="A77" s="3"/>
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
@@ -5422,7 +5428,7 @@
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
     </row>
-    <row r="78" spans="1:29" ht="24.9" customHeight="1">
+    <row r="78" spans="1:32" ht="24.9" customHeight="1">
       <c r="A78" s="3"/>
       <c r="B78" s="19">
         <v>21</v>
@@ -5504,7 +5510,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:29" ht="24.9" customHeight="1">
+    <row r="79" spans="1:32" ht="24.9" customHeight="1">
       <c r="A79" s="3"/>
       <c r="B79" s="19">
         <f>B78+1</f>
@@ -5587,7 +5593,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="1:29" ht="24.9" customHeight="1">
+    <row r="80" spans="1:32" ht="24.9" customHeight="1">
       <c r="A80" s="3"/>
       <c r="B80" s="19">
         <f t="shared" ref="B80:B97" si="3">B79+1</f>

</xml_diff>

<commit_message>
Part as single formula
</commit_message>
<xml_diff>
--- a/Lalaon-teny (Ny Tsiory) - Cas.xlsx
+++ b/Lalaon-teny (Ny Tsiory) - Cas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6361D73-DF2A-49B9-84E0-71702553FB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4110B6-0483-41C0-937E-2E4014D0979D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="626" xr2:uid="{27FFEEF4-A9D8-40D1-B209-21085DC60689}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Plateau" sheetId="47" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_fn">_xlfn.LAMBDA(_xlpm.w,_xlpm.draws,_xlfn.LET(_xlpm.z,MID(_xlpm.w,_xlfn.SEQUENCE(LEN(_xlpm.w)),1), _xlpm.q,_xlfn.GROUPBY(_xlpm.z,_xlpm.z,_xleta.ROWS,0,0), _xlpm.qq,_xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(_xlpm.draws=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq) ))</definedName>
     <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
     <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
     <definedName name="IQ_FWD_CY2" hidden="1">10003</definedName>
@@ -3866,7 +3867,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="728" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="805" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -3884,6 +3885,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -3901,8 +3905,8 @@
   </sheetPr>
   <dimension ref="A1:AT145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A63" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E64" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -5293,6 +5297,13 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J75:AC75=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>18</v>
       </c>
+      <c r="I75" s="1" cm="1">
+        <f t="array" ref="I75">_xlfn.LAMBDA(_xlpm.w,_xlpm.draws,_xlfn.LET(_xlpm.z,MID(_xlpm.w,_xlfn.SEQUENCE(LEN(_xlpm.w)),1),
+_xlpm.q,_xlfn.GROUPBY(_xlpm.z,_xlpm.z,_xleta.ROWS,0,0),
+_xlpm.qq,_xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(_xlpm.draws=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq)
+))(G75,J75:AC75)</f>
+        <v>18</v>
+      </c>
       <c r="J75" s="40" t="s">
         <v>61</v>
       </c>
@@ -5380,6 +5391,10 @@
         <f t="array" ref="H76">_xlfn.LET(_xlpm.z,MID(G76,_xlfn.SEQUENCE(LEN(G76)),1),
      _xlpm.q,  _xlfn.GROUPBY(_xlpm.z,_xlpm.z,_xleta.ROWS,0,0),
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J76:AC76=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
+        <v>6</v>
+      </c>
+      <c r="I76" s="1" cm="1">
+        <f t="array" ref="I76">_fn(G76,J76:AC76)</f>
         <v>6</v>
       </c>
       <c r="J76" s="40" t="s">
@@ -5484,6 +5499,10 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J78:AC78=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>18</v>
       </c>
+      <c r="I78" s="1" cm="1">
+        <f t="array" ref="I78:I97">_xlfn.BYROW(_xlfn.HSTACK(G78:G97,J78:AC97),_xlfn.LAMBDA(_xlpm.r, _xlfn.LET(_xlpm.x,INDEX(_xlpm.r,1,1),_xlpm.draws,_xlfn.DROP(_xlpm.r,,1),_fn(_xlpm.x,_xlpm.draws))))</f>
+        <v>18</v>
+      </c>
       <c r="J78" s="40" t="s">
         <v>63</v>
       </c>
@@ -5570,6 +5589,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J79:AC79=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>20</v>
       </c>
+      <c r="I79" s="1">
+        <v>20</v>
+      </c>
       <c r="J79" s="40" t="s">
         <v>67</v>
       </c>
@@ -5656,6 +5678,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J80:AC80=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>9</v>
       </c>
+      <c r="I80" s="1">
+        <v>9</v>
+      </c>
       <c r="J80" s="40" t="s">
         <v>74</v>
       </c>
@@ -5742,6 +5767,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J81:AC81=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>12</v>
       </c>
+      <c r="I81" s="1">
+        <v>12</v>
+      </c>
       <c r="J81" s="40" t="s">
         <v>78</v>
       </c>
@@ -5828,6 +5856,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J82:AC82=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>19</v>
       </c>
+      <c r="I82" s="1">
+        <v>19</v>
+      </c>
       <c r="J82" s="40" t="s">
         <v>76</v>
       </c>
@@ -5914,6 +5945,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J83:AC83=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>17</v>
       </c>
+      <c r="I83" s="1">
+        <v>17</v>
+      </c>
       <c r="J83" s="40" t="s">
         <v>69</v>
       </c>
@@ -6000,6 +6034,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J84:AC84=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>5</v>
       </c>
+      <c r="I84" s="1">
+        <v>5</v>
+      </c>
       <c r="J84" s="40" t="s">
         <v>76</v>
       </c>
@@ -6086,6 +6123,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J85:AC85=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>18</v>
       </c>
+      <c r="I85" s="1">
+        <v>18</v>
+      </c>
       <c r="J85" s="40" t="s">
         <v>81</v>
       </c>
@@ -6172,6 +6212,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J86:AC86=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>19</v>
       </c>
+      <c r="I86" s="1">
+        <v>19</v>
+      </c>
       <c r="J86" s="40" t="s">
         <v>67</v>
       </c>
@@ -6258,6 +6301,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J87:AC87=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>18</v>
       </c>
+      <c r="I87" s="1">
+        <v>18</v>
+      </c>
       <c r="J87" s="40" t="s">
         <v>61</v>
       </c>
@@ -6344,6 +6390,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J88:AC88=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>19</v>
       </c>
+      <c r="I88" s="1">
+        <v>19</v>
+      </c>
       <c r="J88" s="40" t="s">
         <v>64</v>
       </c>
@@ -6430,6 +6479,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J89:AC89=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>12</v>
       </c>
+      <c r="I89" s="1">
+        <v>12</v>
+      </c>
       <c r="J89" s="40" t="s">
         <v>88</v>
       </c>
@@ -6516,6 +6568,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J90:AC90=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>19</v>
       </c>
+      <c r="I90" s="1">
+        <v>19</v>
+      </c>
       <c r="J90" s="40" t="s">
         <v>75</v>
       </c>
@@ -6602,6 +6657,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J91:AC91=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>19</v>
       </c>
+      <c r="I91" s="1">
+        <v>19</v>
+      </c>
       <c r="J91" s="40" t="s">
         <v>84</v>
       </c>
@@ -6688,6 +6746,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J92:AC92=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>13</v>
       </c>
+      <c r="I92" s="1">
+        <v>13</v>
+      </c>
       <c r="J92" s="40" t="s">
         <v>64</v>
       </c>
@@ -6774,6 +6835,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J93:AC93=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>14</v>
       </c>
+      <c r="I93" s="1">
+        <v>14</v>
+      </c>
       <c r="J93" s="40" t="s">
         <v>94</v>
       </c>
@@ -6860,6 +6924,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J94:AC94=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>12</v>
       </c>
+      <c r="I94" s="1">
+        <v>12</v>
+      </c>
       <c r="J94" s="40" t="s">
         <v>84</v>
       </c>
@@ -6946,6 +7013,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J95:AC95=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>11</v>
       </c>
+      <c r="I95" s="1">
+        <v>11</v>
+      </c>
       <c r="J95" s="40" t="s">
         <v>69</v>
       </c>
@@ -7032,6 +7102,9 @@
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J96:AC96=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
         <v>20</v>
       </c>
+      <c r="I96" s="1">
+        <v>20</v>
+      </c>
       <c r="J96" s="40" t="s">
         <v>70</v>
       </c>
@@ -7116,6 +7189,9 @@
         <f t="array" ref="H97">_xlfn.LET(_xlpm.z,MID(G97,_xlfn.SEQUENCE(LEN(G97)),1),
      _xlpm.q,  _xlfn.GROUPBY(_xlpm.z,_xlpm.z,_xleta.ROWS,0,0),
      _xlpm.qq, _xlfn.BYROW(_xlpm.q,_xlfn.LAMBDA(_xlpm.r,_xlfn.XMATCH(_xlfn.TAKE(_xlpm.r,,-1),_xlfn.SCAN(0,--(J97:AC97=_xlfn.TAKE(_xlpm.r,,1)),_xleta.SUM)))),MAX(_xlpm.qq))</f>
+        <v>16</v>
+      </c>
+      <c r="I97" s="1">
         <v>16</v>
       </c>
       <c r="J97" s="40" t="s">

</xml_diff>

<commit_message>
Start work on part 3
</commit_message>
<xml_diff>
--- a/Lalaon-teny (Ny Tsiory) - Cas.xlsx
+++ b/Lalaon-teny (Ny Tsiory) - Cas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29022"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4110B6-0483-41C0-937E-2E4014D0979D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8C6A9C-3EA2-4CC8-A298-83C4052C6473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="626" xr2:uid="{27FFEEF4-A9D8-40D1-B209-21085DC60689}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="626" xr2:uid="{27FFEEF4-A9D8-40D1-B209-21085DC60689}"/>
   </bookViews>
   <sheets>
     <sheet name="Cas" sheetId="49" r:id="rId1"/>
@@ -3360,7 +3360,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>464344</xdr:colOff>
+      <xdr:colOff>473868</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>151011</xdr:rowOff>
     </xdr:to>
@@ -3403,16 +3403,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>580430</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>297656</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>423552</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>121635</xdr:rowOff>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>434982</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>246055</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3435,8 +3435,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11382375" y="27360563"/>
-          <a:ext cx="14842021" cy="1371791"/>
+          <a:off x="22800469" y="26015156"/>
+          <a:ext cx="15025496" cy="1388579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3454,7 +3454,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>586066</xdr:colOff>
+      <xdr:colOff>593686</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -3905,8 +3905,8 @@
   </sheetPr>
   <dimension ref="A1:AT145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E64" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A95" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K118" sqref="K118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -3918,12 +3918,14 @@
     <col min="5" max="5" width="31.6640625" style="6" customWidth="1"/>
     <col min="6" max="6" width="6.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25" style="1" customWidth="1"/>
-    <col min="8" max="9" width="15.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.21875" style="1" customWidth="1"/>
     <col min="11" max="11" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="15" width="8.5546875" style="3"/>
     <col min="16" max="16" width="10.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="21" width="8.5546875" style="3"/>
+    <col min="17" max="18" width="10.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="8.5546875" style="3"/>
     <col min="22" max="22" width="8.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.88671875" style="3" bestFit="1" customWidth="1"/>
@@ -7334,6 +7336,10 @@
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="2"/>
+      <c r="Q104" s="3" t="str">
+        <f>_xlfn.TRANSLATE(B104,"fr")</f>
+        <v>Words are now placed on the board in a specific direction, starting with the very first character of the word.</v>
+      </c>
     </row>
     <row r="105" spans="1:32" ht="15" customHeight="1">
       <c r="A105" s="3"/>
@@ -7343,6 +7349,10 @@
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="2"/>
+      <c r="Q105" s="3" t="str">
+        <f t="shared" ref="Q105:Q114" si="4">_xlfn.TRANSLATE(B105,"fr")</f>
+        <v>Each question is independent of the others: the board is therefore emptied of all its letters at the beginning of each question.</v>
+      </c>
     </row>
     <row r="106" spans="1:32" ht="15" customHeight="1">
       <c r="A106" s="3"/>
@@ -7352,6 +7362,10 @@
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="2"/>
+      <c r="Q106" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>What is the point value of each word when placed on the board, for each question?</v>
+      </c>
     </row>
     <row r="107" spans="1:32" ht="15" customHeight="1">
       <c r="A107" s="3"/>
@@ -7359,6 +7373,10 @@
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="2"/>
+      <c r="Q107" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
     <row r="108" spans="1:32" ht="15" customHeight="1">
       <c r="A108" s="3"/>
@@ -7368,6 +7386,10 @@
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="2"/>
+      <c r="Q108" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Letter multipliers apply before word multipliers. In other words, if a letter is placed on a Double Letter (LD) square, its value is doubled and then integrated into the calculation of the word before a word multiplier is applied.</v>
+      </c>
     </row>
     <row r="109" spans="1:32" ht="15" customHeight="1">
       <c r="A109" s="3"/>
@@ -7377,6 +7399,10 @@
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="2"/>
+      <c r="Q109" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Word multipliers, on the other hand, are cumulative. For example, if a word spans two Double Word (MD) squares, its total value is multiplied by 4.</v>
+      </c>
     </row>
     <row r="110" spans="1:32" ht="15" customHeight="1">
       <c r="A110" s="3"/>
@@ -7384,6 +7410,10 @@
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="2"/>
+      <c r="Q110" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
     <row r="111" spans="1:32" ht="15" customHeight="1">
       <c r="A111" s="3"/>
@@ -7395,6 +7425,14 @@
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="2"/>
+      <c r="Q111" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>Example3d:</v>
+      </c>
+      <c r="R111" s="3" t="str">
+        <f>_xlfn.TRANSLATE(C111,"fr")</f>
+        <v>The word AKAIKY is placed letter by letter on the following squares: A on F5, K on E5, A on D5, I on C5, K on B5, and Y on A5.</v>
+      </c>
     </row>
     <row r="112" spans="1:32" ht="15" customHeight="1">
       <c r="A112" s="3"/>
@@ -7404,6 +7442,10 @@
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="2"/>
+      <c r="Q112" s="3" t="str">
+        <f>_xlfn.TRANSLATE(C112,"fr")</f>
+        <v>The first K is on a Double Letter (LD) square, the I is on a Triple Word (MT) square and the Y on a Triple Letter (LT) square.</v>
+      </c>
     </row>
     <row r="113" spans="1:25" ht="15" customHeight="1">
       <c r="A113" s="3"/>
@@ -7412,6 +7454,10 @@
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="2"/>
+      <c r="Q113" s="3" t="str">
+        <f t="shared" ref="Q113:Q114" si="5">_xlfn.TRANSLATE(C113,"fr")</f>
+        <v>The calculation of the points is therefore as follows:</v>
+      </c>
     </row>
     <row r="114" spans="1:25" ht="15" customHeight="1">
       <c r="A114" s="3"/>
@@ -7421,15 +7467,45 @@
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="2"/>
+      <c r="Q114" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>(1 + 11*2 + 1 + 1*3 + 11 + 5*3) * 3 = 159 points.</v>
+      </c>
     </row>
     <row r="115" spans="1:25" ht="15" customHeight="1" thickBot="1">
       <c r="A115" s="3"/>
-      <c r="B115" s="16"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="2"/>
-      <c r="H115" s="3"/>
-      <c r="I115" s="3"/>
+      <c r="B115" s="16" t="str">
+        <f>_xlfn.TRANSLATE(B116,"fr")</f>
+        <v>Question #</v>
+      </c>
+      <c r="C115" s="16" t="str">
+        <f t="shared" ref="C115:I115" si="6">_xlfn.TRANSLATE(C116,"fr")</f>
+        <v>Level</v>
+      </c>
+      <c r="D115" s="16" t="str">
+        <f t="shared" si="6"/>
+        <v>Points</v>
+      </c>
+      <c r="E115" s="16" t="str">
+        <f t="shared" si="6"/>
+        <v>Answer</v>
+      </c>
+      <c r="F115" s="16" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="G115" s="16" t="str">
+        <f t="shared" si="6"/>
+        <v>Word</v>
+      </c>
+      <c r="H115" s="16" t="str">
+        <f t="shared" si="6"/>
+        <v>Placement of the first letter</v>
+      </c>
+      <c r="I115" s="16" t="str">
+        <f t="shared" si="6"/>
+        <v>Investment management</v>
+      </c>
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
     </row>
@@ -7643,7 +7719,7 @@
     <row r="124" spans="1:25" ht="35.1" customHeight="1">
       <c r="A124" s="3"/>
       <c r="B124" s="19">
-        <f t="shared" ref="B124:B142" si="4">B123+1</f>
+        <f t="shared" ref="B124:B142" si="7">B123+1</f>
         <v>42</v>
       </c>
       <c r="C124" s="19">
@@ -7675,7 +7751,7 @@
     <row r="125" spans="1:25" ht="35.1" customHeight="1">
       <c r="A125" s="3"/>
       <c r="B125" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
       <c r="C125" s="19">
@@ -7707,7 +7783,7 @@
     <row r="126" spans="1:25" ht="35.1" customHeight="1">
       <c r="A126" s="3"/>
       <c r="B126" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
       <c r="C126" s="19">
@@ -7733,7 +7809,7 @@
     <row r="127" spans="1:25" ht="35.1" customHeight="1">
       <c r="A127" s="3"/>
       <c r="B127" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="C127" s="19">
@@ -7759,7 +7835,7 @@
     <row r="128" spans="1:25" ht="35.1" customHeight="1">
       <c r="A128" s="3"/>
       <c r="B128" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>46</v>
       </c>
       <c r="C128" s="19">
@@ -7785,7 +7861,7 @@
     <row r="129" spans="1:32" ht="35.1" customHeight="1">
       <c r="A129" s="3"/>
       <c r="B129" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>47</v>
       </c>
       <c r="C129" s="19">
@@ -7811,7 +7887,7 @@
     <row r="130" spans="1:32" ht="35.1" customHeight="1">
       <c r="A130" s="3"/>
       <c r="B130" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="C130" s="19">
@@ -7837,7 +7913,7 @@
     <row r="131" spans="1:32" ht="35.1" customHeight="1">
       <c r="A131" s="3"/>
       <c r="B131" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>49</v>
       </c>
       <c r="C131" s="19">
@@ -7863,7 +7939,7 @@
     <row r="132" spans="1:32" ht="35.1" customHeight="1">
       <c r="A132" s="3"/>
       <c r="B132" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
       <c r="C132" s="19">
@@ -7888,7 +7964,7 @@
     <row r="133" spans="1:32" ht="35.1" customHeight="1">
       <c r="A133" s="3"/>
       <c r="B133" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>51</v>
       </c>
       <c r="C133" s="19">
@@ -7913,7 +7989,7 @@
     <row r="134" spans="1:32" ht="35.1" customHeight="1">
       <c r="A134" s="3"/>
       <c r="B134" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>52</v>
       </c>
       <c r="C134" s="19">
@@ -7938,7 +8014,7 @@
     <row r="135" spans="1:32" ht="35.1" customHeight="1">
       <c r="A135" s="3"/>
       <c r="B135" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>53</v>
       </c>
       <c r="C135" s="19">
@@ -7963,7 +8039,7 @@
     <row r="136" spans="1:32" ht="35.1" customHeight="1">
       <c r="A136" s="3"/>
       <c r="B136" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>54</v>
       </c>
       <c r="C136" s="19">
@@ -7988,7 +8064,7 @@
     <row r="137" spans="1:32" ht="35.1" customHeight="1">
       <c r="A137" s="3"/>
       <c r="B137" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>55</v>
       </c>
       <c r="C137" s="19">
@@ -8013,7 +8089,7 @@
     <row r="138" spans="1:32" ht="35.1" customHeight="1">
       <c r="A138" s="3"/>
       <c r="B138" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>56</v>
       </c>
       <c r="C138" s="19">
@@ -8038,7 +8114,7 @@
     <row r="139" spans="1:32" ht="35.1" customHeight="1">
       <c r="A139" s="3"/>
       <c r="B139" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>57</v>
       </c>
       <c r="C139" s="19">
@@ -8063,7 +8139,7 @@
     <row r="140" spans="1:32" ht="35.1" customHeight="1">
       <c r="A140" s="3"/>
       <c r="B140" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>58</v>
       </c>
       <c r="C140" s="19">
@@ -8088,7 +8164,7 @@
     <row r="141" spans="1:32" ht="35.1" customHeight="1">
       <c r="A141" s="3"/>
       <c r="B141" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>59</v>
       </c>
       <c r="C141" s="19">
@@ -8113,7 +8189,7 @@
     <row r="142" spans="1:32" ht="35.1" customHeight="1">
       <c r="A142" s="3"/>
       <c r="B142" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="C142" s="19">
@@ -8438,7 +8514,7 @@
   </sheetPr>
   <dimension ref="B2:F653"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A553" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A541" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -13818,18 +13894,21 @@
   <sheetPr>
     <tabColor rgb="FF006837"/>
   </sheetPr>
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="60" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="60" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3:X6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="15" width="7.5546875" customWidth="1"/>
     <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="42" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="36.6">
+    <row r="1" spans="1:24" ht="36.6">
       <c r="A1" s="57" t="s">
         <v>768</v>
       </c>
@@ -13856,7 +13935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="36.6">
+    <row r="2" spans="1:24" ht="36.6">
       <c r="A2" s="62"/>
       <c r="B2" s="59" t="s">
         <v>770</v>
@@ -13892,7 +13971,7 @@
       </c>
       <c r="U2" s="75"/>
     </row>
-    <row r="3" spans="1:21" ht="36.6">
+    <row r="3" spans="1:24" ht="36.6">
       <c r="A3" s="62"/>
       <c r="B3" s="60" t="s">
         <v>771</v>
@@ -13929,8 +14008,12 @@
       <c r="U3" s="77" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="36.6">
+      <c r="X3" t="str">
+        <f>_xlfn.TRANSLATE(U3,"fr")</f>
+        <v>Multiply the value of the letter placed on it by 2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="36.6">
       <c r="A4" s="62"/>
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
@@ -13965,8 +14048,12 @@
       <c r="U4" s="78" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="36.6">
+      <c r="X4" t="str">
+        <f t="shared" ref="X4:X6" si="0">_xlfn.TRANSLATE(U4,"fr")</f>
+        <v>Multiply the value of the letter placed on it by 3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="36.6">
       <c r="A5" s="58" t="s">
         <v>769</v>
       </c>
@@ -14003,8 +14090,12 @@
       <c r="U5" s="78" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="36.6">
+      <c r="X5" t="str">
+        <f t="shared" si="0"/>
+        <v>Multiply the value of the word placed on it by 2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="36.6">
       <c r="A6" s="62"/>
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
@@ -14037,8 +14128,12 @@
       <c r="U6" s="78" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="36.6">
+      <c r="X6" t="str">
+        <f t="shared" si="0"/>
+        <v>Multiply the value of the word placed on it by 3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="36.6">
       <c r="A7" s="62"/>
       <c r="B7" s="62"/>
       <c r="C7" s="62"/>
@@ -14063,7 +14158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="36.6">
+    <row r="8" spans="1:24" ht="36.6">
       <c r="A8" s="58" t="s">
         <v>769</v>
       </c>
@@ -14094,7 +14189,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="36.6">
+    <row r="9" spans="1:24" ht="36.6">
       <c r="A9" s="62"/>
       <c r="B9" s="62"/>
       <c r="C9" s="62"/>
@@ -14119,7 +14214,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="36.6">
+    <row r="10" spans="1:24" ht="36.6">
       <c r="A10" s="62"/>
       <c r="B10" s="62"/>
       <c r="C10" s="62"/>
@@ -14144,7 +14239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="36.6">
+    <row r="11" spans="1:24" ht="36.6">
       <c r="A11" s="62"/>
       <c r="B11" s="62"/>
       <c r="C11" s="62"/>
@@ -14173,7 +14268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="36.6">
+    <row r="12" spans="1:24" ht="36.6">
       <c r="A12" s="62"/>
       <c r="B12" s="62"/>
       <c r="C12" s="62"/>
@@ -14198,7 +14293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="36.6">
+    <row r="13" spans="1:24" ht="36.6">
       <c r="A13" s="62"/>
       <c r="B13" s="60" t="s">
         <v>771</v>
@@ -14227,7 +14322,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="36.6">
+    <row r="14" spans="1:24" ht="36.6">
       <c r="A14" s="62"/>
       <c r="B14" s="59" t="s">
         <v>770</v>
@@ -14256,7 +14351,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="36.6">
+    <row r="15" spans="1:24" ht="36.6">
       <c r="A15" s="59" t="s">
         <v>770</v>
       </c>
@@ -14285,7 +14380,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="25.8">
+    <row r="16" spans="1:24" ht="25.8">
       <c r="A16" s="61" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
working on my solution of problem 3
</commit_message>
<xml_diff>
--- a/Lalaon-teny (Ny Tsiory) - Cas.xlsx
+++ b/Lalaon-teny (Ny Tsiory) - Cas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29022"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29024"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8C6A9C-3EA2-4CC8-A298-83C4052C6473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41D81AE-548A-41D9-A826-32D5EF47CBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="626" xr2:uid="{27FFEEF4-A9D8-40D1-B209-21085DC60689}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="784">
   <si>
     <t>Lalaon-teny</t>
   </si>
@@ -2438,6 +2438,12 @@
   </si>
   <si>
     <t>Multiplier la valeur du mot placé dessus par 3</t>
+  </si>
+  <si>
+    <t>Letter Value</t>
+  </si>
+  <si>
+    <t>Word Multiplier</t>
   </si>
 </sst>
 </file>
@@ -2768,7 +2774,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -3089,13 +3095,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3316,6 +3406,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink 2" xfId="1" xr:uid="{9C19BEA1-C844-4C71-AF9A-880BFE097251}"/>
@@ -3360,7 +3480,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>473868</xdr:colOff>
+      <xdr:colOff>477678</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>151011</xdr:rowOff>
     </xdr:to>
@@ -3410,9 +3530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>53</xdr:col>
-      <xdr:colOff>434982</xdr:colOff>
+      <xdr:colOff>438792</xdr:colOff>
       <xdr:row>98</xdr:row>
-      <xdr:rowOff>246055</xdr:rowOff>
+      <xdr:rowOff>249865</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3454,7 +3574,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>593686</xdr:colOff>
+      <xdr:colOff>589876</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -3489,6 +3609,77 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>14</xdr:col>
+          <xdr:colOff>365760</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>137160</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>19</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Picture 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F64EFFBE-C30B-1A0F-8809-C0781EE554D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="Cas!$Q$114:$T$114" spid="_x0000_s3076"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="7620000" y="7650480"/>
+              <a:ext cx="2674620" cy="198120"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -3905,8 +4096,8 @@
   </sheetPr>
   <dimension ref="A1:AT145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A95" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K118" sqref="K118"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -7350,7 +7541,7 @@
       <c r="D105" s="1"/>
       <c r="E105" s="2"/>
       <c r="Q105" s="3" t="str">
-        <f t="shared" ref="Q105:Q114" si="4">_xlfn.TRANSLATE(B105,"fr")</f>
+        <f t="shared" ref="Q105:Q111" si="4">_xlfn.TRANSLATE(B105,"fr")</f>
         <v>Each question is independent of the others: the board is therefore emptied of all its letters at the beginning of each question.</v>
       </c>
     </row>
@@ -7603,7 +7794,6 @@
       <c r="M119" s="14"/>
       <c r="N119" s="14"/>
       <c r="O119" s="14"/>
-      <c r="P119" s="14"/>
       <c r="Q119" s="14"/>
     </row>
     <row r="120" spans="1:25" ht="35.1" customHeight="1">
@@ -8514,7 +8704,7 @@
   </sheetPr>
   <dimension ref="B2:F653"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A541" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -13890,14 +14080,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5012A788-1D60-415A-AB01-CB76C5B6EDAD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5012A788-1D60-415A-AB01-CB76C5B6EDAD}">
   <sheetPr>
     <tabColor rgb="FF006837"/>
   </sheetPr>
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="60" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3:X6"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -13905,6 +14095,7 @@
     <col min="1" max="15" width="7.5546875" customWidth="1"/>
     <col min="20" max="20" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="42" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.77734375" customWidth="1"/>
     <col min="24" max="24" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14008,20 +14199,24 @@
       <c r="U3" s="77" t="s">
         <v>775</v>
       </c>
+      <c r="W3" t="str">
+        <f>_xlfn.TRANSLATE(T3,"fr")</f>
+        <v>Double Letter</v>
+      </c>
       <c r="X3" t="str">
         <f>_xlfn.TRANSLATE(U3,"fr")</f>
         <v>Multiply the value of the letter placed on it by 2</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="36.6">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="59" t="s">
+    <row r="4" spans="1:24" ht="37.200000000000003" thickBot="1">
+      <c r="A4" s="85"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="86" t="s">
         <v>770</v>
       </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
       <c r="G4" s="62"/>
       <c r="H4" s="58" t="s">
         <v>769</v>
@@ -14048,25 +14243,29 @@
       <c r="U4" s="78" t="s">
         <v>777</v>
       </c>
+      <c r="W4" t="str">
+        <f t="shared" ref="W4:W6" si="0">_xlfn.TRANSLATE(T4,"fr")</f>
+        <v>Triple Letter</v>
+      </c>
       <c r="X4" t="str">
-        <f t="shared" ref="X4:X6" si="0">_xlfn.TRANSLATE(U4,"fr")</f>
+        <f t="shared" ref="X4:X6" si="1">_xlfn.TRANSLATE(U4,"fr")</f>
         <v>Multiply the value of the letter placed on it by 3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="36.6">
-      <c r="A5" s="58" t="s">
+    <row r="5" spans="1:24" ht="37.799999999999997" thickTop="1" thickBot="1">
+      <c r="A5" s="89" t="s">
         <v>769</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="57" t="s">
+      <c r="B5" s="90"/>
+      <c r="C5" s="91" t="s">
         <v>768</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="59" t="s">
+      <c r="D5" s="90"/>
+      <c r="E5" s="92" t="s">
         <v>770</v>
       </c>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="84"/>
       <c r="H5" s="62"/>
       <c r="I5" s="62"/>
       <c r="J5" s="62"/>
@@ -14090,18 +14289,22 @@
       <c r="U5" s="78" t="s">
         <v>779</v>
       </c>
+      <c r="W5" t="str">
+        <f t="shared" si="0"/>
+        <v>Double Word</v>
+      </c>
       <c r="X5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Multiply the value of the word placed on it by 2</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="36.6">
-      <c r="A6" s="62"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="59" t="s">
+    <row r="6" spans="1:24" ht="37.200000000000003" thickTop="1">
+      <c r="A6" s="87"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="88" t="s">
         <v>770</v>
       </c>
       <c r="G6" s="62"/>
@@ -14128,8 +14331,12 @@
       <c r="U6" s="78" t="s">
         <v>781</v>
       </c>
+      <c r="W6" t="str">
+        <f t="shared" si="0"/>
+        <v>Triple Word</v>
+      </c>
       <c r="X6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Multiply the value of the word placed on it by 3</v>
       </c>
     </row>
@@ -14427,8 +14634,130 @@
         <v>78</v>
       </c>
     </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="56">
+        <f>_xlfn.XLOOKUP(A19,'Mots et Lettres'!$E$5:$E$30,'Mots et Lettres'!$F$5:$F$30)</f>
+        <v>5</v>
+      </c>
+      <c r="B18" s="56">
+        <f>_xlfn.XLOOKUP(B19,'Mots et Lettres'!$E$5:$E$30,'Mots et Lettres'!$F$5:$F$30)</f>
+        <v>11</v>
+      </c>
+      <c r="C18" s="56">
+        <f>_xlfn.XLOOKUP(C19,'Mots et Lettres'!$E$5:$E$30,'Mots et Lettres'!$F$5:$F$30)</f>
+        <v>3</v>
+      </c>
+      <c r="D18" s="56">
+        <f>_xlfn.XLOOKUP(D19,'Mots et Lettres'!$E$5:$E$30,'Mots et Lettres'!$F$5:$F$30)</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="56">
+        <f>_xlfn.XLOOKUP(E19,'Mots et Lettres'!$E$5:$E$30,'Mots et Lettres'!$F$5:$F$30)</f>
+        <v>11</v>
+      </c>
+      <c r="F18" s="56">
+        <f>_xlfn.XLOOKUP(F19,'Mots et Lettres'!$E$5:$E$30,'Mots et Lettres'!$F$5:$F$30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="56">
+        <v>3</v>
+      </c>
+      <c r="B20" s="56">
+        <v>1</v>
+      </c>
+      <c r="C20" s="56">
+        <v>1</v>
+      </c>
+      <c r="D20" s="56">
+        <v>1</v>
+      </c>
+      <c r="E20" s="56">
+        <v>2</v>
+      </c>
+      <c r="F20" s="56">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f>SUMPRODUCT(A20:F20,A18:F18)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="56">
+        <f t="shared" ref="A21:E21" si="2">A18*A20</f>
+        <v>15</v>
+      </c>
+      <c r="B21" s="56">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="C21" s="56">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D21" s="56">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="56">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="F21" s="56">
+        <f>F18*F20</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="56">
+        <f>SUM(A21:F21)</f>
+        <v>53</v>
+      </c>
+      <c r="I21" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="G23">
+        <f>G21*H22</f>
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Breaking down Problem 3
</commit_message>
<xml_diff>
--- a/Lalaon-teny (Ny Tsiory) - Cas.xlsx
+++ b/Lalaon-teny (Ny Tsiory) - Cas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41D81AE-548A-41D9-A826-32D5EF47CBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024170DB-7D86-4E59-8E41-3268808A7E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="626" xr2:uid="{27FFEEF4-A9D8-40D1-B209-21085DC60689}"/>
   </bookViews>
@@ -3480,7 +3480,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>477678</xdr:colOff>
+      <xdr:colOff>473868</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>151011</xdr:rowOff>
     </xdr:to>
@@ -3530,9 +3530,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>53</xdr:col>
-      <xdr:colOff>438792</xdr:colOff>
+      <xdr:colOff>434982</xdr:colOff>
       <xdr:row>98</xdr:row>
-      <xdr:rowOff>249865</xdr:rowOff>
+      <xdr:rowOff>246055</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3574,7 +3574,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>589876</xdr:colOff>
+      <xdr:colOff>593686</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -3619,15 +3619,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>365760</xdr:colOff>
+          <xdr:colOff>361950</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>19</xdr:col>
-          <xdr:colOff>142875</xdr:colOff>
+          <xdr:colOff>183356</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:rowOff>152202</xdr:rowOff>
         </xdr:to>
         <xdr:pic>
           <xdr:nvPicPr>
@@ -3642,7 +3642,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Cas!$Q$114:$T$114" spid="_x0000_s3076"/>
+                  <a14:cameraTool cellRange="Cas!$Q$114:$T$114" spid="_x0000_s3078"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3656,8 +3656,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="7620000" y="7650480"/>
-              <a:ext cx="2674620" cy="198120"/>
+              <a:off x="7473950" y="7578725"/>
+              <a:ext cx="2678906" cy="193477"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -4096,8 +4096,8 @@
   </sheetPr>
   <dimension ref="A1:AT145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G119" sqref="G119"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="64" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M118" sqref="M118:M121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -4113,7 +4113,9 @@
     <col min="9" max="9" width="15.44140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.21875" style="1" customWidth="1"/>
     <col min="11" max="11" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="8.5546875" style="3"/>
+    <col min="12" max="12" width="8.5546875" style="3"/>
+    <col min="13" max="13" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8.5546875" style="3"/>
     <col min="16" max="16" width="10.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="10.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="21" width="8.5546875" style="3"/>
@@ -7638,7 +7640,7 @@
         <v>The first K is on a Double Letter (LD) square, the I is on a Triple Word (MT) square and the Y on a Triple Letter (LT) square.</v>
       </c>
     </row>
-    <row r="113" spans="1:25" ht="15" customHeight="1">
+    <row r="113" spans="1:26" ht="15" customHeight="1">
       <c r="A113" s="3"/>
       <c r="C113" s="16" t="s">
         <v>121</v>
@@ -7650,7 +7652,7 @@
         <v>The calculation of the points is therefore as follows:</v>
       </c>
     </row>
-    <row r="114" spans="1:25" ht="15" customHeight="1">
+    <row r="114" spans="1:26" ht="15" customHeight="1">
       <c r="A114" s="3"/>
       <c r="B114" s="10"/>
       <c r="C114" s="1" t="s">
@@ -7663,7 +7665,7 @@
         <v>(1 + 11*2 + 1 + 1*3 + 11 + 5*3) * 3 = 159 points.</v>
       </c>
     </row>
-    <row r="115" spans="1:25" ht="15" customHeight="1" thickBot="1">
+    <row r="115" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A115" s="3"/>
       <c r="B115" s="16" t="str">
         <f>_xlfn.TRANSLATE(B116,"fr")</f>
@@ -7700,7 +7702,7 @@
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
     </row>
-    <row r="116" spans="1:25" ht="39" customHeight="1" thickTop="1" thickBot="1">
+    <row r="116" spans="1:26" ht="39" customHeight="1" thickTop="1" thickBot="1">
       <c r="A116" s="3"/>
       <c r="B116" s="18" t="s">
         <v>10</v>
@@ -7726,7 +7728,7 @@
       <c r="J116" s="3"/>
       <c r="K116" s="3"/>
     </row>
-    <row r="117" spans="1:25" ht="15" thickTop="1">
+    <row r="117" spans="1:26" ht="15" thickTop="1">
       <c r="A117" s="3"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -7737,7 +7739,7 @@
       <c r="J117" s="3"/>
       <c r="K117" s="3"/>
     </row>
-    <row r="118" spans="1:25" ht="35.1" customHeight="1">
+    <row r="118" spans="1:26" ht="35.1" customHeight="1">
       <c r="A118" s="3"/>
       <c r="B118" s="19" t="s">
         <v>125</v>
@@ -7762,9 +7764,59 @@
         <v>128</v>
       </c>
       <c r="J118" s="3"/>
-      <c r="K118" s="3"/>
-    </row>
-    <row r="119" spans="1:25" ht="35.1" customHeight="1">
+      <c r="K118" s="3">
+        <f>CODE(LEFT(H118,1))-CODE("A")+1</f>
+        <v>1</v>
+      </c>
+      <c r="L118" s="3">
+        <f>MID(H118,2,100)+0</f>
+        <v>1</v>
+      </c>
+      <c r="M118" s="3" t="str" cm="1">
+        <f t="array" ref="M118:Z118">_xlfn.LET(_xlpm.n,LEN(G118),_xlfn.SWITCH(TRUE,I118="→",CHAR(K118+CODE("A")+_xlfn.SEQUENCE(1,_xlpm.n)-2)&amp;L118,I118="←",CHAR(K118+CODE("A")+_xlfn.SEQUENCE(1,_xlpm.n)-2)&amp;L118,I118="↑", CHAR(CODE("A")-1+K118)&amp;_xlfn.SEQUENCE(1,_xlpm.n,L118,-1),I118="↓",CHAR(CODE("A")-1+K118)&amp;_xlfn.SEQUENCE(1,_xlpm.n,L118,1)))</f>
+        <v>A1</v>
+      </c>
+      <c r="N118" s="3" t="str">
+        <v>B1</v>
+      </c>
+      <c r="O118" s="3" t="str">
+        <v>C1</v>
+      </c>
+      <c r="P118" s="3" t="str">
+        <v>D1</v>
+      </c>
+      <c r="Q118" s="3" t="str">
+        <v>E1</v>
+      </c>
+      <c r="R118" s="3" t="str">
+        <v>F1</v>
+      </c>
+      <c r="S118" s="3" t="str">
+        <v>G1</v>
+      </c>
+      <c r="T118" s="3" t="str">
+        <v>H1</v>
+      </c>
+      <c r="U118" s="3" t="str">
+        <v>I1</v>
+      </c>
+      <c r="V118" s="3" t="str">
+        <v>J1</v>
+      </c>
+      <c r="W118" s="3" t="str">
+        <v>K1</v>
+      </c>
+      <c r="X118" s="3" t="str">
+        <v>L1</v>
+      </c>
+      <c r="Y118" s="3" t="str">
+        <v>M1</v>
+      </c>
+      <c r="Z118" s="3" t="str">
+        <v>N1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:26" ht="35.1" customHeight="1">
       <c r="A119" s="3"/>
       <c r="B119" s="19" t="s">
         <v>129</v>
@@ -7789,14 +7841,44 @@
         <v>132</v>
       </c>
       <c r="J119" s="14"/>
-      <c r="K119" s="14"/>
-      <c r="L119" s="14"/>
-      <c r="M119" s="14"/>
-      <c r="N119" s="14"/>
-      <c r="O119" s="14"/>
-      <c r="Q119" s="14"/>
-    </row>
-    <row r="120" spans="1:25" ht="35.1" customHeight="1">
+      <c r="K119" s="3">
+        <f t="shared" ref="K119:K121" si="7">CODE(LEFT(H119,1))-CODE("A")+1</f>
+        <v>12</v>
+      </c>
+      <c r="L119" s="3">
+        <f t="shared" ref="L119:L121" si="8">MID(H119,2,100)+0</f>
+        <v>13</v>
+      </c>
+      <c r="M119" s="3" t="str" cm="1">
+        <f t="array" ref="M119:U119">_xlfn.LET(_xlpm.n,LEN(G119),_xlfn.SWITCH(TRUE,I119="→",CHAR(K119+CODE("A")+_xlfn.SEQUENCE(1,_xlpm.n)-2)&amp;L119,I119="←",CHAR(K119+CODE("A")+_xlfn.SEQUENCE(1,_xlpm.n)-2)&amp;L119,I119="↑", CHAR(CODE("A")-1+K119)&amp;_xlfn.SEQUENCE(1,_xlpm.n,L119,-1),I119="↓",CHAR(CODE("A")-1+K119)&amp;_xlfn.SEQUENCE(1,_xlpm.n,L119,1)))</f>
+        <v>L13</v>
+      </c>
+      <c r="N119" s="14" t="str">
+        <v>L12</v>
+      </c>
+      <c r="O119" s="14" t="str">
+        <v>L11</v>
+      </c>
+      <c r="P119" s="3" t="str">
+        <v>L10</v>
+      </c>
+      <c r="Q119" s="14" t="str">
+        <v>L9</v>
+      </c>
+      <c r="R119" s="3" t="str">
+        <v>L8</v>
+      </c>
+      <c r="S119" s="3" t="str">
+        <v>L7</v>
+      </c>
+      <c r="T119" s="3" t="str">
+        <v>L6</v>
+      </c>
+      <c r="U119" s="3" t="str">
+        <v>L5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:26" ht="35.1" customHeight="1">
       <c r="A120" s="3"/>
       <c r="B120" s="19" t="s">
         <v>133</v>
@@ -7821,17 +7903,52 @@
         <v>136</v>
       </c>
       <c r="J120" s="14"/>
-      <c r="K120" s="3"/>
-      <c r="L120" s="14"/>
-      <c r="M120" s="14"/>
-      <c r="T120"/>
-      <c r="U120"/>
-      <c r="V120"/>
-      <c r="W120"/>
+      <c r="K120" s="3">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="L120" s="3">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="M120" s="3" t="str" cm="1">
+        <f t="array" ref="M120:W120">_xlfn.LET(_xlpm.n,LEN(G120),_xlfn.SWITCH(TRUE,I120="→",CHAR(K120+CODE("A")+_xlfn.SEQUENCE(1,_xlpm.n)-2)&amp;L120,I120="←",CHAR(K120+CODE("A")+_xlfn.SEQUENCE(1,_xlpm.n)-2)&amp;L120,I120="↑", CHAR(CODE("A")-1+K120)&amp;_xlfn.SEQUENCE(1,_xlpm.n,L120,-1),I120="↓",CHAR(CODE("A")-1+K120)&amp;_xlfn.SEQUENCE(1,_xlpm.n,L120,1)))</f>
+        <v>D4</v>
+      </c>
+      <c r="N120" s="3" t="str">
+        <v>D5</v>
+      </c>
+      <c r="O120" s="3" t="str">
+        <v>D6</v>
+      </c>
+      <c r="P120" s="3" t="str">
+        <v>D7</v>
+      </c>
+      <c r="Q120" s="3" t="str">
+        <v>D8</v>
+      </c>
+      <c r="R120" s="3" t="str">
+        <v>D9</v>
+      </c>
+      <c r="S120" s="3" t="str">
+        <v>D10</v>
+      </c>
+      <c r="T120" t="str">
+        <v>D11</v>
+      </c>
+      <c r="U120" t="str">
+        <v>D12</v>
+      </c>
+      <c r="V120" t="str">
+        <v>D13</v>
+      </c>
+      <c r="W120" t="str">
+        <v>D14</v>
+      </c>
       <c r="X120"/>
       <c r="Y120"/>
     </row>
-    <row r="121" spans="1:25" ht="35.1" customHeight="1">
+    <row r="121" spans="1:26" ht="35.1" customHeight="1">
       <c r="A121" s="3"/>
       <c r="B121" s="19" t="s">
         <v>137</v>
@@ -7856,15 +7973,35 @@
         <v>140</v>
       </c>
       <c r="J121" s="14"/>
-      <c r="K121" s="14"/>
-      <c r="L121" s="14"/>
-      <c r="M121" s="14"/>
-      <c r="N121" s="14"/>
-      <c r="O121" s="14"/>
-      <c r="P121" s="14"/>
-      <c r="Q121" s="14"/>
-    </row>
-    <row r="122" spans="1:25">
+      <c r="K121" s="3">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="L121" s="3">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="M121" s="3" t="str" cm="1">
+        <f t="array" ref="M121:R121">_xlfn.LET(_xlpm.n,LEN(G121),_xlfn.SWITCH(TRUE,I121="→",CHAR(K121+CODE("A")+_xlfn.SEQUENCE(1,_xlpm.n)-2)&amp;L121,I121="←",CHAR(K121+CODE("A")+_xlfn.SEQUENCE(1,_xlpm.n)-2)&amp;L121,I121="↑", CHAR(CODE("A")-1+K121)&amp;_xlfn.SEQUENCE(1,_xlpm.n,L121,-1),I121="↓",CHAR(CODE("A")-1+K121)&amp;_xlfn.SEQUENCE(1,_xlpm.n,L121,1)))</f>
+        <v>F5</v>
+      </c>
+      <c r="N121" s="14" t="str">
+        <v>G5</v>
+      </c>
+      <c r="O121" s="14" t="str">
+        <v>H5</v>
+      </c>
+      <c r="P121" s="14" t="str">
+        <v>I5</v>
+      </c>
+      <c r="Q121" s="14" t="str">
+        <v>J5</v>
+      </c>
+      <c r="R121" s="3" t="str">
+        <v>K5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:26">
       <c r="A122" s="3"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -7875,7 +8012,7 @@
       <c r="J122" s="3"/>
       <c r="K122" s="3"/>
     </row>
-    <row r="123" spans="1:25" ht="35.1" customHeight="1">
+    <row r="123" spans="1:26" ht="35.1" customHeight="1">
       <c r="A123" s="3"/>
       <c r="B123" s="19">
         <v>41</v>
@@ -7906,10 +8043,10 @@
       <c r="P123" s="14"/>
       <c r="Q123" s="14"/>
     </row>
-    <row r="124" spans="1:25" ht="35.1" customHeight="1">
+    <row r="124" spans="1:26" ht="35.1" customHeight="1">
       <c r="A124" s="3"/>
       <c r="B124" s="19">
-        <f t="shared" ref="B124:B142" si="7">B123+1</f>
+        <f t="shared" ref="B124:B142" si="9">B123+1</f>
         <v>42</v>
       </c>
       <c r="C124" s="19">
@@ -7938,10 +8075,10 @@
       <c r="P124" s="14"/>
       <c r="Q124" s="14"/>
     </row>
-    <row r="125" spans="1:25" ht="35.1" customHeight="1">
+    <row r="125" spans="1:26" ht="35.1" customHeight="1">
       <c r="A125" s="3"/>
       <c r="B125" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>43</v>
       </c>
       <c r="C125" s="19">
@@ -7970,10 +8107,10 @@
       <c r="P125" s="14"/>
       <c r="Q125" s="14"/>
     </row>
-    <row r="126" spans="1:25" ht="35.1" customHeight="1">
+    <row r="126" spans="1:26" ht="35.1" customHeight="1">
       <c r="A126" s="3"/>
       <c r="B126" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>44</v>
       </c>
       <c r="C126" s="19">
@@ -7996,10 +8133,10 @@
       <c r="J126" s="14"/>
       <c r="K126" s="3"/>
     </row>
-    <row r="127" spans="1:25" ht="35.1" customHeight="1">
+    <row r="127" spans="1:26" ht="35.1" customHeight="1">
       <c r="A127" s="3"/>
       <c r="B127" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="C127" s="19">
@@ -8022,10 +8159,10 @@
       <c r="J127" s="14"/>
       <c r="K127" s="3"/>
     </row>
-    <row r="128" spans="1:25" ht="35.1" customHeight="1">
+    <row r="128" spans="1:26" ht="35.1" customHeight="1">
       <c r="A128" s="3"/>
       <c r="B128" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>46</v>
       </c>
       <c r="C128" s="19">
@@ -8051,7 +8188,7 @@
     <row r="129" spans="1:32" ht="35.1" customHeight="1">
       <c r="A129" s="3"/>
       <c r="B129" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>47</v>
       </c>
       <c r="C129" s="19">
@@ -8077,7 +8214,7 @@
     <row r="130" spans="1:32" ht="35.1" customHeight="1">
       <c r="A130" s="3"/>
       <c r="B130" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>48</v>
       </c>
       <c r="C130" s="19">
@@ -8103,7 +8240,7 @@
     <row r="131" spans="1:32" ht="35.1" customHeight="1">
       <c r="A131" s="3"/>
       <c r="B131" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>49</v>
       </c>
       <c r="C131" s="19">
@@ -8129,7 +8266,7 @@
     <row r="132" spans="1:32" ht="35.1" customHeight="1">
       <c r="A132" s="3"/>
       <c r="B132" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="C132" s="19">
@@ -8154,7 +8291,7 @@
     <row r="133" spans="1:32" ht="35.1" customHeight="1">
       <c r="A133" s="3"/>
       <c r="B133" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>51</v>
       </c>
       <c r="C133" s="19">
@@ -8179,7 +8316,7 @@
     <row r="134" spans="1:32" ht="35.1" customHeight="1">
       <c r="A134" s="3"/>
       <c r="B134" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>52</v>
       </c>
       <c r="C134" s="19">
@@ -8204,7 +8341,7 @@
     <row r="135" spans="1:32" ht="35.1" customHeight="1">
       <c r="A135" s="3"/>
       <c r="B135" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>53</v>
       </c>
       <c r="C135" s="19">
@@ -8229,7 +8366,7 @@
     <row r="136" spans="1:32" ht="35.1" customHeight="1">
       <c r="A136" s="3"/>
       <c r="B136" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>54</v>
       </c>
       <c r="C136" s="19">
@@ -8254,7 +8391,7 @@
     <row r="137" spans="1:32" ht="35.1" customHeight="1">
       <c r="A137" s="3"/>
       <c r="B137" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>55</v>
       </c>
       <c r="C137" s="19">
@@ -8279,7 +8416,7 @@
     <row r="138" spans="1:32" ht="35.1" customHeight="1">
       <c r="A138" s="3"/>
       <c r="B138" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>56</v>
       </c>
       <c r="C138" s="19">
@@ -8304,7 +8441,7 @@
     <row r="139" spans="1:32" ht="35.1" customHeight="1">
       <c r="A139" s="3"/>
       <c r="B139" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>57</v>
       </c>
       <c r="C139" s="19">
@@ -8329,7 +8466,7 @@
     <row r="140" spans="1:32" ht="35.1" customHeight="1">
       <c r="A140" s="3"/>
       <c r="B140" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>58</v>
       </c>
       <c r="C140" s="19">
@@ -8354,7 +8491,7 @@
     <row r="141" spans="1:32" ht="35.1" customHeight="1">
       <c r="A141" s="3"/>
       <c r="B141" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="C141" s="19">
@@ -8379,7 +8516,7 @@
     <row r="142" spans="1:32" ht="35.1" customHeight="1">
       <c r="A142" s="3"/>
       <c r="B142" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="C142" s="19">

</xml_diff>